<commit_message>
various updates to report structure.
</commit_message>
<xml_diff>
--- a/tabular/contributed/180718 SOF TABLE b.xlsx
+++ b/tabular/contributed/180718 SOF TABLE b.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="1180" windowWidth="37940" windowHeight="27280"/>
+    <workbookView xWindow="6960" yWindow="3120" windowWidth="37940" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="SOF new" sheetId="3" r:id="rId1"/>
@@ -848,6 +848,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -857,7 +858,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1162,9 +1162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3600,7 +3600,7 @@
       <c r="I55" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J55" s="37" t="s">
+      <c r="J55" s="34" t="s">
         <v>192</v>
       </c>
       <c r="K55" s="16" t="s">
@@ -3643,7 +3643,7 @@
       <c r="I56" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J56" s="37" t="s">
+      <c r="J56" s="34" t="s">
         <v>192</v>
       </c>
       <c r="K56" s="16" t="s">
@@ -3686,7 +3686,7 @@
       <c r="I57" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J57" s="37" t="s">
+      <c r="J57" s="34" t="s">
         <v>192</v>
       </c>
       <c r="K57" s="16" t="s">
@@ -5930,7 +5930,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
-      <c r="B2" s="34"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
@@ -5938,29 +5938,29 @@
         <v>14</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="34"/>
+      <c r="G2" s="35"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="35" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -5970,7 +5970,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
@@ -5978,15 +5978,15 @@
         <v>18</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="34"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="35"/>
       <c r="O3" s="3" t="s">
         <v>24</v>
       </c>

</xml_diff>